<commit_message>
Medians for all parameters
</commit_message>
<xml_diff>
--- a/out_anuch.xlsx
+++ b/out_anuch.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="161" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="188" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="out_anuch" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="192">
   <si>
     <t>May</t>
   </si>
@@ -23,7 +23,7 @@
     <t>nan</t>
   </si>
   <si>
-    <t>10.5181451613</t>
+    <t>9.7</t>
   </si>
   <si>
     <t>27.1</t>
@@ -32,7 +32,7 @@
     <t>0.2</t>
   </si>
   <si>
-    <t>67.4796747967</t>
+    <t>70.0</t>
   </si>
   <si>
     <t>100.0</t>
@@ -41,7 +41,7 @@
     <t>15.0</t>
   </si>
   <si>
-    <t>5.975</t>
+    <t>3.0</t>
   </si>
   <si>
     <t>25.0</t>
@@ -50,7 +50,7 @@
     <t>0.3</t>
   </si>
   <si>
-    <t>13.8723577236</t>
+    <t>13.4</t>
   </si>
   <si>
     <t>29.8</t>
@@ -59,7 +59,7 @@
     <t>1.1</t>
   </si>
   <si>
-    <t>60.0326530612</t>
+    <t>61.0</t>
   </si>
   <si>
     <t>99.0</t>
@@ -68,13 +68,13 @@
     <t>16.0</t>
   </si>
   <si>
-    <t>2.48</t>
+    <t>2.0</t>
   </si>
   <si>
     <t>12.0</t>
   </si>
   <si>
-    <t>12.4384615385</t>
+    <t>11.6</t>
   </si>
   <si>
     <t>29.6</t>
@@ -83,61 +83,43 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>67.5263157895</t>
-  </si>
-  <si>
-    <t>4.27</t>
-  </si>
-  <si>
     <t>19.0</t>
   </si>
   <si>
-    <t>11.9123404255</t>
-  </si>
-  <si>
     <t>25.2</t>
   </si>
   <si>
-    <t>71.2936170213</t>
+    <t>75.0</t>
   </si>
   <si>
     <t>18.0</t>
   </si>
   <si>
-    <t>3.19433962264</t>
-  </si>
-  <si>
     <t>0.1</t>
   </si>
   <si>
-    <t>14.6955284553</t>
+    <t>14.2</t>
   </si>
   <si>
     <t>30.8</t>
   </si>
   <si>
-    <t>55.8244897959</t>
-  </si>
-  <si>
-    <t>4.06666666667</t>
+    <t>55.0</t>
   </si>
   <si>
     <t>13.0</t>
   </si>
   <si>
-    <t>13.8346774194</t>
+    <t>13.1</t>
   </si>
   <si>
     <t>30.4</t>
   </si>
   <si>
-    <t>62.3064516129</t>
-  </si>
-  <si>
-    <t>3.548</t>
-  </si>
-  <si>
-    <t>11.7008064516</t>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>10.55</t>
   </si>
   <si>
     <t>27.0</t>
@@ -146,16 +128,13 @@
     <t>0.0</t>
   </si>
   <si>
-    <t>68.2701612903</t>
-  </si>
-  <si>
-    <t>4.20952380952</t>
+    <t>74.0</t>
   </si>
   <si>
     <t>22.0</t>
   </si>
   <si>
-    <t>13.697983871</t>
+    <t>12.45</t>
   </si>
   <si>
     <t>29.2</t>
@@ -164,13 +143,10 @@
     <t>4.1</t>
   </si>
   <si>
-    <t>67.963562753</t>
-  </si>
-  <si>
-    <t>2.46444444444</t>
-  </si>
-  <si>
-    <t>14.0241935484</t>
+    <t>71.0</t>
+  </si>
+  <si>
+    <t>12.85</t>
   </si>
   <si>
     <t>32.5</t>
@@ -179,7 +155,7 @@
     <t>2.3</t>
   </si>
   <si>
-    <t>65.3209876543</t>
+    <t>68.0</t>
   </si>
   <si>
     <t>98.0</t>
@@ -188,13 +164,10 @@
     <t>11.0</t>
   </si>
   <si>
-    <t>4.05263157895</t>
-  </si>
-  <si>
     <t>24.0</t>
   </si>
   <si>
-    <t>13.1564516129</t>
+    <t>12.2</t>
   </si>
   <si>
     <t>32.2</t>
@@ -203,16 +176,10 @@
     <t>-0.3</t>
   </si>
   <si>
-    <t>68.5967741935</t>
-  </si>
-  <si>
     <t>14.0</t>
   </si>
   <si>
-    <t>5.15925925926</t>
-  </si>
-  <si>
-    <t>13.2080645161</t>
+    <t>12.25</t>
   </si>
   <si>
     <t>30.9</t>
@@ -221,13 +188,10 @@
     <t>-0.1</t>
   </si>
   <si>
-    <t>62.8306451613</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
-    <t>3.35</t>
+    <t>2.5</t>
   </si>
   <si>
     <t>17.0</t>
@@ -236,7 +200,7 @@
     <t>July</t>
   </si>
   <si>
-    <t>20.2139830508</t>
+    <t>19.7</t>
   </si>
   <si>
     <t>31.6</t>
@@ -245,19 +209,16 @@
     <t>12.6</t>
   </si>
   <si>
-    <t>83.0595744681</t>
+    <t>88.0</t>
   </si>
   <si>
     <t>39.0</t>
   </si>
   <si>
-    <t>8.93055555556</t>
-  </si>
-  <si>
     <t>29.0</t>
   </si>
   <si>
-    <t>21.170781893</t>
+    <t>20.5</t>
   </si>
   <si>
     <t>32.6</t>
@@ -266,10 +227,7 @@
     <t>9.9</t>
   </si>
   <si>
-    <t>76.6255144033</t>
-  </si>
-  <si>
-    <t>5.45714285714</t>
+    <t>82.0</t>
   </si>
   <si>
     <t>37.0</t>
@@ -278,7 +236,7 @@
     <t>0.4</t>
   </si>
   <si>
-    <t>19.743852459</t>
+    <t>19.25</t>
   </si>
   <si>
     <t>33.1</t>
@@ -287,19 +245,16 @@
     <t>1.7</t>
   </si>
   <si>
-    <t>75.8765432099</t>
+    <t>80.0</t>
   </si>
   <si>
     <t>31.0</t>
   </si>
   <si>
-    <t>5.69090909091</t>
-  </si>
-  <si>
     <t>0.6</t>
   </si>
   <si>
-    <t>21.7552742616</t>
+    <t>20.7</t>
   </si>
   <si>
     <t>33.3</t>
@@ -308,49 +263,40 @@
     <t>12.8</t>
   </si>
   <si>
-    <t>81.5654008439</t>
-  </si>
-  <si>
-    <t>6.7875</t>
+    <t>87.0</t>
   </si>
   <si>
     <t>40.0</t>
   </si>
   <si>
-    <t>19.6232653061</t>
-  </si>
-  <si>
     <t>-13.8</t>
   </si>
   <si>
-    <t>83.5226337449</t>
-  </si>
-  <si>
-    <t>6.825</t>
-  </si>
-  <si>
-    <t>21.5361788618</t>
+    <t>89.0</t>
+  </si>
+  <si>
+    <t>8.0</t>
+  </si>
+  <si>
+    <t>21.35</t>
   </si>
   <si>
     <t>31.7</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>83.4938271605</t>
+    <t>86.0</t>
   </si>
   <si>
     <t>47.0</t>
   </si>
   <si>
-    <t>5.95208333333</t>
+    <t>4.0</t>
   </si>
   <si>
     <t>30.0</t>
   </si>
   <si>
-    <t>21.9942622951</t>
+    <t>21.5</t>
   </si>
   <si>
     <t>32.8</t>
@@ -359,28 +305,22 @@
     <t>11.3</t>
   </si>
   <si>
-    <t>80.6818181818</t>
-  </si>
-  <si>
-    <t>11.8166666667</t>
+    <t>84.0</t>
   </si>
   <si>
     <t>60.0</t>
   </si>
   <si>
-    <t>21.6205645161</t>
-  </si>
-  <si>
-    <t>79.2186234818</t>
+    <t>83.0</t>
   </si>
   <si>
     <t>35.0</t>
   </si>
   <si>
-    <t>5.28235294118</t>
-  </si>
-  <si>
-    <t>21.7</t>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>20.9</t>
   </si>
   <si>
     <t>32.3</t>
@@ -389,22 +329,16 @@
     <t>13.6</t>
   </si>
   <si>
-    <t>78.5236220472</t>
-  </si>
-  <si>
     <t>96.0</t>
   </si>
   <si>
     <t>28.0</t>
   </si>
   <si>
-    <t>8.7</t>
-  </si>
-  <si>
     <t>32.0</t>
   </si>
   <si>
-    <t>21.6846774194</t>
+    <t>21.3</t>
   </si>
   <si>
     <t>31.2</t>
@@ -413,13 +347,13 @@
     <t>13.3</t>
   </si>
   <si>
-    <t>73.7177419355</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>21.025</t>
+    <t>76.0</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>20.6</t>
   </si>
   <si>
     <t>33.4</t>
@@ -428,31 +362,28 @@
     <t>10.9</t>
   </si>
   <si>
-    <t>75.6370967742</t>
-  </si>
-  <si>
-    <t>8.125</t>
+    <t>79.5</t>
   </si>
   <si>
     <t>June</t>
   </si>
   <si>
-    <t>19.0179166667</t>
+    <t>18.2</t>
   </si>
   <si>
     <t>10.0</t>
   </si>
   <si>
-    <t>76.2166666667</t>
-  </si>
-  <si>
-    <t>2.27857142857</t>
+    <t>81.0</t>
+  </si>
+  <si>
+    <t>1.5</t>
   </si>
   <si>
     <t>6.0</t>
   </si>
   <si>
-    <t>16.9567226891</t>
+    <t>16.7</t>
   </si>
   <si>
     <t>26.8</t>
@@ -461,16 +392,13 @@
     <t>8.6</t>
   </si>
   <si>
-    <t>76.5991561181</t>
+    <t>79.0</t>
   </si>
   <si>
     <t>36.0</t>
   </si>
   <si>
-    <t>2.88205128205</t>
-  </si>
-  <si>
-    <t>18.83</t>
+    <t>17.95</t>
   </si>
   <si>
     <t>33.5</t>
@@ -479,16 +407,13 @@
     <t>7.5</t>
   </si>
   <si>
-    <t>70.4791666667</t>
-  </si>
-  <si>
-    <t>2.70416666667</t>
+    <t>74.5</t>
   </si>
   <si>
     <t>7.0</t>
   </si>
   <si>
-    <t>17.9679324895</t>
+    <t>17.5</t>
   </si>
   <si>
     <t>32.4</t>
@@ -497,16 +422,10 @@
     <t>6.5</t>
   </si>
   <si>
-    <t>72.6822033898</t>
-  </si>
-  <si>
-    <t>6.075</t>
-  </si>
-  <si>
     <t>0.5</t>
   </si>
   <si>
-    <t>16.2265822785</t>
+    <t>16.1</t>
   </si>
   <si>
     <t>30.6</t>
@@ -515,13 +434,7 @@
     <t>6.9</t>
   </si>
   <si>
-    <t>75.9324894515</t>
-  </si>
-  <si>
-    <t>4.71333333333</t>
-  </si>
-  <si>
-    <t>20.8847457627</t>
+    <t>20.55</t>
   </si>
   <si>
     <t>36.2</t>
@@ -530,58 +443,40 @@
     <t>9.4</t>
   </si>
   <si>
-    <t>71.5720338983</t>
+    <t>76.5</t>
   </si>
   <si>
     <t>23.0</t>
   </si>
   <si>
-    <t>4.90967741935</t>
+    <t>0.8</t>
   </si>
   <si>
     <t>48.0</t>
   </si>
   <si>
-    <t>17.4941422594</t>
+    <t>16.4</t>
   </si>
   <si>
     <t>7.6</t>
   </si>
   <si>
-    <t>75.9288702929</t>
-  </si>
-  <si>
-    <t>4.14418604651</t>
-  </si>
-  <si>
-    <t>17.7683333333</t>
+    <t>16.8</t>
   </si>
   <si>
     <t>30.3</t>
   </si>
   <si>
-    <t>77.6945606695</t>
-  </si>
-  <si>
     <t>26.0</t>
   </si>
   <si>
-    <t>3.62857142857</t>
-  </si>
-  <si>
-    <t>18.8995833333</t>
-  </si>
-  <si>
-    <t>71.4791666667</t>
+    <t>17.75</t>
   </si>
   <si>
     <t>97.0</t>
   </si>
   <si>
-    <t>4.38461538462</t>
-  </si>
-  <si>
-    <t>19.02375</t>
+    <t>17.3</t>
   </si>
   <si>
     <t>35.3</t>
@@ -590,13 +485,7 @@
     <t>10.1</t>
   </si>
   <si>
-    <t>74.7666666667</t>
-  </si>
-  <si>
-    <t>3.12352941176</t>
-  </si>
-  <si>
-    <t>17.8979166667</t>
+    <t>16.9</t>
   </si>
   <si>
     <t>31.4</t>
@@ -605,133 +494,82 @@
     <t>7.7</t>
   </si>
   <si>
-    <t>73.4708333333</t>
-  </si>
-  <si>
-    <t>7.16666666667</t>
+    <t>78.5</t>
+  </si>
+  <si>
+    <t>4.5</t>
   </si>
   <si>
     <t>August</t>
   </si>
   <si>
-    <t>20.7163934426</t>
-  </si>
-  <si>
     <t>11.4</t>
   </si>
   <si>
-    <t>82.7745901639</t>
-  </si>
-  <si>
-    <t>5.07692307692</t>
+    <t>90.0</t>
   </si>
   <si>
     <t>38.0</t>
   </si>
   <si>
-    <t>21.8064777328</t>
-  </si>
-  <si>
     <t>31.9</t>
   </si>
   <si>
-    <t>82.9306122449</t>
-  </si>
-  <si>
     <t>43.0</t>
   </si>
   <si>
-    <t>4.7380952381</t>
-  </si>
-  <si>
-    <t>21.8817073171</t>
-  </si>
-  <si>
     <t>1.6</t>
   </si>
   <si>
-    <t>76.5040983607</t>
-  </si>
-  <si>
     <t>21.0</t>
   </si>
   <si>
-    <t>4.45714285714</t>
-  </si>
-  <si>
-    <t>20.2975308642</t>
-  </si>
-  <si>
-    <t>78.2975206612</t>
-  </si>
-  <si>
-    <t>2.92727272727</t>
-  </si>
-  <si>
-    <t>20.0028688525</t>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>84.5</t>
+  </si>
+  <si>
+    <t>19.6</t>
   </si>
   <si>
     <t>6.3</t>
   </si>
   <si>
-    <t>79.0286885246</t>
-  </si>
-  <si>
-    <t>4.74705882353</t>
-  </si>
-  <si>
-    <t>22.0766129032</t>
+    <t>85.0</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>21.8</t>
   </si>
   <si>
     <t>14.1</t>
   </si>
   <si>
-    <t>82.4534412955</t>
-  </si>
-  <si>
     <t>41.0</t>
   </si>
   <si>
-    <t>5.475</t>
-  </si>
-  <si>
     <t>33.0</t>
   </si>
   <si>
-    <t>21.2316872428</t>
-  </si>
-  <si>
     <t>12.5</t>
   </si>
   <si>
-    <t>81.8888888889</t>
-  </si>
-  <si>
     <t>42.0</t>
   </si>
   <si>
-    <t>6.37837837838</t>
-  </si>
-  <si>
-    <t>20.6291497976</t>
-  </si>
-  <si>
     <t>30.7</t>
   </si>
   <si>
     <t>10.2</t>
   </si>
   <si>
-    <t>83.6923076923</t>
-  </si>
-  <si>
-    <t>11.5954545455</t>
-  </si>
-  <si>
     <t>52.0</t>
   </si>
   <si>
-    <t>21.1842741935</t>
+    <t>21.2</t>
   </si>
   <si>
     <t>31.1</t>
@@ -740,40 +578,19 @@
     <t>9.8</t>
   </si>
   <si>
-    <t>80.5685483871</t>
-  </si>
-  <si>
-    <t>4.6</t>
-  </si>
-  <si>
-    <t>20.2149193548</t>
+    <t>19.3</t>
   </si>
   <si>
     <t>32.9</t>
   </si>
   <si>
-    <t>77.2822580645</t>
-  </si>
-  <si>
-    <t>7.92142857143</t>
-  </si>
-  <si>
     <t>20.0</t>
   </si>
   <si>
-    <t>21.0489878543</t>
-  </si>
-  <si>
     <t>34.4</t>
   </si>
   <si>
     <t>11.1</t>
-  </si>
-  <si>
-    <t>78.995951417</t>
-  </si>
-  <si>
-    <t>4.172</t>
   </si>
 </sst>
 </file>
@@ -781,12 +598,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
-      <name val="arial"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -814,7 +631,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -823,43 +640,43 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -871,31 +688,31 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.09183673469388"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.10204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.10204081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.09183673469388"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="5.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.53571428571429"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.10204081632653"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.53571428571429"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2004</v>
       </c>
@@ -927,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2005</v>
       </c>
@@ -959,7 +776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2006</v>
       </c>
@@ -991,7 +808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>2007</v>
       </c>
@@ -1005,7 +822,7 @@
         <v>21</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>6</v>
@@ -1014,62 +831,62 @@
         <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>2008</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>15</v>
@@ -1078,30 +895,30 @@
         <v>18</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>15</v>
@@ -1110,181 +927,181 @@
         <v>18</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>2004</v>
       </c>
@@ -1316,364 +1133,364 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>2006</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>2007</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>92</v>
+        <v>8</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>2008</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>98</v>
+        <v>8</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>7</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>106</v>
+        <v>17</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="J21" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="J22" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="I26" s="0" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="J26" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>2004</v>
       </c>
@@ -1705,62 +1522,62 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="F29" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>2006</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="F30" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>18</v>
@@ -1769,85 +1586,85 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>2007</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="F31" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>155</v>
+        <v>8</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>2008</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="F32" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>161</v>
+        <v>8</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>9</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>15</v>
@@ -1856,7 +1673,7 @@
         <v>9</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>16</v>
@@ -1865,149 +1682,149 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>178</v>
+        <v>17</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J35" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>181</v>
+        <v>70</v>
       </c>
       <c r="F36" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="C37" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>186</v>
-      </c>
       <c r="G37" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>191</v>
+        <v>119</v>
       </c>
       <c r="F38" s="0" t="s">
         <v>6</v>
@@ -2016,53 +1833,53 @@
         <v>7</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>193</v>
+        <v>156</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>194</v>
+        <v>157</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>195</v>
+        <v>158</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>196</v>
+        <v>159</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>197</v>
+        <v>160</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>2004</v>
       </c>
@@ -2094,365 +1911,365 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>2005</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>199</v>
+        <v>101</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="F42" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="J42" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>2006</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>204</v>
+        <v>107</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>208</v>
+        <v>17</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>9</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>2007</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>209</v>
+        <v>38</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>211</v>
+        <v>98</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>212</v>
+        <v>168</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>213</v>
+        <v>17</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J44" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>2008</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>216</v>
+        <v>21</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="J45" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="46">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>2009</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>217</v>
+        <v>171</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>218</v>
+        <v>172</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>219</v>
+        <v>173</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>220</v>
+        <v>174</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J46" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="47">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>2010</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>221</v>
+        <v>175</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>222</v>
+        <v>176</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>223</v>
+        <v>82</v>
       </c>
       <c r="F47" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>225</v>
+        <v>17</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
       <c r="J47" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="48">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>2011</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>227</v>
+        <v>101</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>228</v>
+        <v>179</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>229</v>
+        <v>85</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>231</v>
+        <v>8</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>2012</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>232</v>
+        <v>112</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>234</v>
+        <v>182</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>235</v>
+        <v>85</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>236</v>
+        <v>121</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>237</v>
+        <v>183</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>2013</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>238</v>
+        <v>184</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>239</v>
+        <v>185</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>240</v>
+        <v>186</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>241</v>
+        <v>82</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>242</v>
+        <v>8</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="J50" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="51">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>2014</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>243</v>
+        <v>187</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>244</v>
+        <v>188</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>234</v>
+        <v>182</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>245</v>
+        <v>173</v>
       </c>
       <c r="F51" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>246</v>
+        <v>134</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
       <c r="J51" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>2015</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>248</v>
+        <v>79</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>249</v>
+        <v>190</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>250</v>
+        <v>191</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>251</v>
+        <v>173</v>
       </c>
       <c r="F52" s="0" t="s">
         <v>6</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>252</v>
+        <v>8</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Tinos,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Tinos,Обычный"&amp;12Страница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>